<commit_message>
new file my account, rc all
</commit_message>
<xml_diff>
--- a/Backlog Task.xlsx
+++ b/Backlog Task.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D765031E-5F8B-41B2-B778-FF223C4C719A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B350BA7-1159-4F19-99D2-3EF2C66D5E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="540" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feature Source" sheetId="2" r:id="rId1"/>
@@ -643,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A581C534-1824-4228-AD4A-6C5848F0268E}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -870,12 +870,15 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A8:D8"/>
@@ -888,15 +891,12 @@
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -906,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -927,7 +927,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
quick create file to the matrix
</commit_message>
<xml_diff>
--- a/Backlog Task.xlsx
+++ b/Backlog Task.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B350BA7-1159-4F19-99D2-3EF2C66D5E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDF28C1-A9F3-4681-A9AF-7F64795B7170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="540" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feature Source" sheetId="2" r:id="rId1"/>
     <sheet name="Test Summary" sheetId="1" r:id="rId2"/>
+    <sheet name="Test Target" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Total  testcase Written</t>
   </si>
@@ -122,6 +123,30 @@
   </si>
   <si>
     <t>Spint( 31 ) - Test Case Summary                                  (6-11-23 -- 12-11-23)</t>
+  </si>
+  <si>
+    <t>Spint( 32 ) - Day 2 - Test Case Summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Written</t>
+  </si>
+  <si>
+    <t>Execution</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>Spint( 32 )</t>
+  </si>
+  <si>
+    <t>20 / (0)</t>
+  </si>
+  <si>
+    <t>40 / (0)</t>
+  </si>
+  <si>
+    <t>40 / (17)</t>
   </si>
 </sst>
 </file>
@@ -644,7 +669,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:D11"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -870,15 +895,12 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A8:D8"/>
@@ -891,12 +913,15 @@
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -904,10 +929,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:C9"/>
+  <dimension ref="B1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -980,12 +1005,95 @@
         <v>0</v>
       </c>
     </row>
+    <row r="14" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="11"/>
+    </row>
+    <row r="15" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B16" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="3">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1339504-D6F3-4F61-92FE-E9AECBD23C71}">
+  <dimension ref="D4:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="D4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="4:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="D5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="D6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="4:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="D7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
change in the pff history...
</commit_message>
<xml_diff>
--- a/Backlog Task.xlsx
+++ b/Backlog Task.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6792BCD-B151-4F4A-8D10-3217F76BA322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0164AA07-A630-4EED-BDD3-08E5EDA5B6DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -904,15 +904,12 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A8:D8"/>
@@ -925,12 +922,15 @@
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1115,7 +1115,7 @@
         <v>0</v>
       </c>
       <c r="C35" s="1">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="18" x14ac:dyDescent="0.3">
@@ -1123,7 +1123,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="2">
-        <v>1</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="18" x14ac:dyDescent="0.3">
@@ -1131,7 +1131,7 @@
         <v>29</v>
       </c>
       <c r="C37" s="3">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chase the previous days...
</commit_message>
<xml_diff>
--- a/Backlog Task.xlsx
+++ b/Backlog Task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0164AA07-A630-4EED-BDD3-08E5EDA5B6DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FE1E94-D283-44B2-9719-FF43DFDFD84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>Total  testcase Written</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>Spint( 33) - Day 2- Test Case Summary</t>
+  </si>
+  <si>
+    <t>Spint( 33) - Day 5- Test Case Summary</t>
   </si>
 </sst>
 </file>
@@ -904,12 +907,15 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A8:D8"/>
@@ -922,15 +928,12 @@
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -938,10 +941,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:C37"/>
+  <dimension ref="B1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1134,8 +1137,39 @@
         <v>20</v>
       </c>
     </row>
+    <row r="41" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B41" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" s="11"/>
+    </row>
+    <row r="42" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B42" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B43" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B44" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" s="3">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="B41:C41"/>
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B6:C6"/>

</xml_diff>

<commit_message>
add api test case first...
</commit_message>
<xml_diff>
--- a/Backlog Task.xlsx
+++ b/Backlog Task.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FE1E94-D283-44B2-9719-FF43DFDFD84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF76E0C-B5D8-4E89-9E14-CA0D64B48982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>Total  testcase Written</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>Spint( 33) - Day 5- Test Case Summary</t>
+  </si>
+  <si>
+    <t>Spint( 34) - Day 5- Test Case Summary</t>
   </si>
 </sst>
 </file>
@@ -941,10 +944,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:C44"/>
+  <dimension ref="B1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="N40" sqref="N40"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1167,8 +1170,39 @@
         <v>20</v>
       </c>
     </row>
+    <row r="47" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B47" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" s="11"/>
+    </row>
+    <row r="48" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B48" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B49" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B50" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" s="3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="B47:C47"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="B1:C1"/>

</xml_diff>

<commit_message>
first commit start windows
</commit_message>
<xml_diff>
--- a/Backlog Task.xlsx
+++ b/Backlog Task.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DA41F3-4426-4CAC-A40F-DE9F2FEC4454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B64EC10-725F-433C-9FE2-6E9E3A322CFF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feature Source" sheetId="2" r:id="rId1"/>
@@ -689,16 +689,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A581C534-1824-4228-AD4A-6C5848F0268E}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>20</v>
       </c>
@@ -706,7 +706,7 @@
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
     </row>
-    <row r="2" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>21</v>
       </c>
@@ -714,7 +714,7 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
     </row>
-    <row r="3" spans="1:4" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>22</v>
       </c>
@@ -722,7 +722,7 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>23</v>
       </c>
@@ -730,7 +730,7 @@
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
     </row>
-    <row r="5" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>24</v>
       </c>
@@ -738,7 +738,7 @@
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
     </row>
-    <row r="6" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>25</v>
       </c>
@@ -746,7 +746,7 @@
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
     </row>
-    <row r="7" spans="1:4" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>26</v>
       </c>
@@ -754,7 +754,7 @@
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>27</v>
       </c>
@@ -762,7 +762,7 @@
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>28</v>
       </c>
@@ -770,7 +770,7 @@
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
@@ -778,7 +778,7 @@
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
     </row>
-    <row r="11" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>3</v>
       </c>
@@ -786,7 +786,7 @@
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>4</v>
       </c>
@@ -794,7 +794,7 @@
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
     </row>
-    <row r="13" spans="1:4" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>5</v>
       </c>
@@ -802,7 +802,7 @@
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>6</v>
       </c>
@@ -810,7 +810,7 @@
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
     </row>
-    <row r="15" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>7</v>
       </c>
@@ -818,7 +818,7 @@
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
     </row>
-    <row r="16" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>8</v>
       </c>
@@ -826,7 +826,7 @@
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
     </row>
-    <row r="17" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>9</v>
       </c>
@@ -834,7 +834,7 @@
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
     </row>
-    <row r="18" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>10</v>
       </c>
@@ -842,7 +842,7 @@
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
     </row>
-    <row r="19" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>11</v>
       </c>
@@ -850,7 +850,7 @@
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
     </row>
-    <row r="20" spans="1:4" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>12</v>
       </c>
@@ -858,7 +858,7 @@
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
     </row>
-    <row r="21" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>13</v>
       </c>
@@ -866,7 +866,7 @@
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
     </row>
-    <row r="22" spans="1:4" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>14</v>
       </c>
@@ -874,7 +874,7 @@
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
     </row>
-    <row r="23" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>15</v>
       </c>
@@ -882,7 +882,7 @@
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
     </row>
-    <row r="24" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>16</v>
       </c>
@@ -890,7 +890,7 @@
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
     </row>
-    <row r="25" spans="1:4" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>17</v>
       </c>
@@ -898,7 +898,7 @@
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
     </row>
-    <row r="26" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>18</v>
       </c>
@@ -906,7 +906,7 @@
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
     </row>
-    <row r="27" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>19</v>
       </c>
@@ -916,15 +916,12 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A8:D8"/>
@@ -937,12 +934,15 @@
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -952,23 +952,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+    <sheetView topLeftCell="A42" workbookViewId="0">
       <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="10" t="s">
         <v>31</v>
       </c>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="2:3" ht="36" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -976,7 +976,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
@@ -984,7 +984,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>29</v>
       </c>
@@ -992,17 +992,17 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
     </row>
-    <row r="6" spans="2:3" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="11"/>
     </row>
-    <row r="7" spans="2:3" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>0</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>1</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>29</v>
       </c>
@@ -1026,13 +1026,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="11"/>
     </row>
-    <row r="15" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>0</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>1</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>29</v>
       </c>
@@ -1056,13 +1056,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="11"/>
     </row>
-    <row r="23" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>0</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>1</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>29</v>
       </c>
@@ -1086,13 +1086,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
         <v>41</v>
       </c>
       <c r="C28" s="11"/>
     </row>
-    <row r="29" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>0</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>1</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>29</v>
       </c>
@@ -1116,13 +1116,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="s">
         <v>42</v>
       </c>
       <c r="C34" s="11"/>
     </row>
-    <row r="35" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>0</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
         <v>1</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>29</v>
       </c>
@@ -1146,13 +1146,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B41" s="10" t="s">
         <v>43</v>
       </c>
       <c r="C41" s="11"/>
     </row>
-    <row r="42" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>0</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
         <v>1</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>29</v>
       </c>
@@ -1176,13 +1176,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B47" s="10" t="s">
         <v>44</v>
       </c>
       <c r="C47" s="11"/>
     </row>
-    <row r="48" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
         <v>0</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B49" s="6" t="s">
         <v>1</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
         <v>29</v>
       </c>
@@ -1206,13 +1206,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B54" s="10" t="s">
         <v>45</v>
       </c>
       <c r="C54" s="11"/>
     </row>
-    <row r="55" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
         <v>0</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="56" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
         <v>1</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="57" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
         <v>29</v>
       </c>
@@ -1236,13 +1236,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B60" s="10" t="s">
         <v>46</v>
       </c>
       <c r="C60" s="11"/>
     </row>
-    <row r="61" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B61" s="5" t="s">
         <v>0</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="62" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B62" s="6" t="s">
         <v>1</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
         <v>29</v>
       </c>
@@ -1268,16 +1268,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B28:C28"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B28:C28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1292,19 +1292,19 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D4" s="10" t="s">
         <v>36</v>
       </c>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="4:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D5" s="5" t="s">
         <v>33</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="4:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D6" s="6" t="s">
         <v>34</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="4:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D7" s="3" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
created and executed test cases for logout and redeem voucher
</commit_message>
<xml_diff>
--- a/Backlog Task.xlsx
+++ b/Backlog Task.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B64EC10-725F-433C-9FE2-6E9E3A322CFF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21BF72DD-B1CF-4287-AAC1-918D591BDA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -916,12 +916,15 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A8:D8"/>
@@ -934,15 +937,12 @@
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1268,16 +1268,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B34:C34"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B34:C34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>